<commit_message>
Added numberofmin changes in same excel file
</commit_message>
<xml_diff>
--- a/Discovery.xlsx
+++ b/Discovery.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIX STREAM1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56B712DE-A9E0-40E6-91F6-D90431B68D44}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AAC982-69AF-4371-99B9-D6A3EA579D4F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10332" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Number of Devices</t>
   </si>
@@ -193,12 +193,105 @@
   </si>
   <si>
     <t>NCEW2 SWAP AVG (MB)</t>
+  </si>
+  <si>
+    <t>DeviceCount</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 2 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 4 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 6 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 8 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 10 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 12 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 14 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 16 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 18 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 20 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 22 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 24 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 26 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 28 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 30 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 32 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 34 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 36 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 38 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 40 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 42 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 44 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 46 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 48 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 50 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 52 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 54 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 56 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 58 min</t>
+  </si>
+  <si>
+    <t>InventoryStatus After 60 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
@@ -241,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -335,6 +428,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -349,7 +481,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -371,15 +503,19 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Excel Built-in Normal 1" xfId="2"/>
-    <cellStyle name="Heading" xfId="3"/>
-    <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="5"/>
-    <cellStyle name="Result2" xfId="6"/>
+    <cellStyle name="Result" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Result2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -690,25 +826,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.75" style="5" customWidth="1"/>
+    <col min="1" max="1" width="32.69921875" style="5" customWidth="1"/>
     <col min="2" max="3" width="11" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.75" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" style="5" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.69921875" style="5" customWidth="1"/>
     <col min="8" max="9" width="15" style="5" customWidth="1"/>
-    <col min="10" max="1023" width="10.75" style="5" customWidth="1"/>
-    <col min="1024" max="1024" width="10.75" customWidth="1"/>
+    <col min="10" max="1023" width="10.69921875" style="5" customWidth="1"/>
+    <col min="1024" max="1024" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +863,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -745,7 +881,7 @@
       <c r="M2"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -763,7 +899,7 @@
       <c r="M3"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -781,7 +917,7 @@
       <c r="M4"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -799,7 +935,7 @@
       <c r="M5"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -817,7 +953,7 @@
       <c r="M6"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -835,7 +971,7 @@
       <c r="M7"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -853,7 +989,7 @@
       <c r="M8"/>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -871,7 +1007,7 @@
       <c r="M9"/>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -889,7 +1025,7 @@
       <c r="M10"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -907,7 +1043,7 @@
       <c r="M11"/>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -925,7 +1061,7 @@
       <c r="M12"/>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -943,7 +1079,7 @@
       <c r="M13"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -961,7 +1097,7 @@
       <c r="M14"/>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -979,7 +1115,7 @@
       <c r="M15"/>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -997,7 +1133,7 @@
       <c r="M16"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1015,7 +1151,7 @@
       <c r="M17"/>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1033,7 +1169,7 @@
       <c r="M18"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
@@ -1051,7 +1187,7 @@
       <c r="M19"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1069,7 +1205,7 @@
       <c r="M20"/>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>15</v>
       </c>
@@ -1087,7 +1223,7 @@
       <c r="M21"/>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -1105,7 +1241,7 @@
       <c r="M22"/>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
@@ -1123,7 +1259,7 @@
       <c r="M23"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1277,7 @@
       <c r="M24"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -1159,7 +1295,7 @@
       <c r="M25"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -1177,7 +1313,7 @@
       <c r="M26"/>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
@@ -1195,7 +1331,7 @@
       <c r="M27"/>
       <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
@@ -1213,7 +1349,7 @@
       <c r="M28"/>
       <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -1231,7 +1367,7 @@
       <c r="M29"/>
       <c r="O29" s="8"/>
     </row>
-    <row r="30" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
@@ -1249,7 +1385,7 @@
       <c r="M30"/>
       <c r="O30" s="8"/>
     </row>
-    <row r="31" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -1267,7 +1403,7 @@
       <c r="M31"/>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -1285,7 +1421,7 @@
       <c r="M32"/>
       <c r="O32" s="8"/>
     </row>
-    <row r="33" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
@@ -1303,7 +1439,7 @@
       <c r="M33"/>
       <c r="O33" s="8"/>
     </row>
-    <row r="34" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1457,7 @@
       <c r="M34"/>
       <c r="O34" s="8"/>
     </row>
-    <row r="35" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
@@ -1339,7 +1475,7 @@
       <c r="M35"/>
       <c r="O35" s="8"/>
     </row>
-    <row r="36" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>36</v>
       </c>
@@ -1357,7 +1493,7 @@
       <c r="M36"/>
       <c r="O36" s="8"/>
     </row>
-    <row r="37" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1375,7 +1511,7 @@
       <c r="M37"/>
       <c r="O37" s="8"/>
     </row>
-    <row r="38" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>38</v>
       </c>
@@ -1393,7 +1529,7 @@
       <c r="M38"/>
       <c r="O38" s="8"/>
     </row>
-    <row r="39" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -1411,7 +1547,7 @@
       <c r="M39"/>
       <c r="O39" s="8"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -1429,7 +1565,7 @@
       <c r="M40"/>
       <c r="O40" s="8"/>
     </row>
-    <row r="41" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>41</v>
       </c>
@@ -1447,7 +1583,7 @@
       <c r="M41"/>
       <c r="O41" s="8"/>
     </row>
-    <row r="42" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1465,7 +1601,7 @@
       <c r="M42"/>
       <c r="O42" s="8"/>
     </row>
-    <row r="43" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
@@ -1483,7 +1619,7 @@
       <c r="M43"/>
       <c r="O43" s="8"/>
     </row>
-    <row r="44" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -1501,7 +1637,7 @@
       <c r="M44"/>
       <c r="O44" s="8"/>
     </row>
-    <row r="45" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -1519,7 +1655,7 @@
       <c r="M45"/>
       <c r="O45" s="8"/>
     </row>
-    <row r="46" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -1537,7 +1673,7 @@
       <c r="M46"/>
       <c r="O46" s="8"/>
     </row>
-    <row r="47" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -1555,7 +1691,7 @@
       <c r="M47"/>
       <c r="O47" s="8"/>
     </row>
-    <row r="48" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
@@ -1573,7 +1709,7 @@
       <c r="M48"/>
       <c r="O48" s="8"/>
     </row>
-    <row r="49" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
@@ -1591,7 +1727,7 @@
       <c r="M49"/>
       <c r="O49" s="8"/>
     </row>
-    <row r="50" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -1609,7 +1745,7 @@
       <c r="M50"/>
       <c r="O50" s="8"/>
     </row>
-    <row r="51" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -1627,7 +1763,7 @@
       <c r="M51"/>
       <c r="O51" s="8"/>
     </row>
-    <row r="52" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -1645,7 +1781,7 @@
       <c r="M52"/>
       <c r="O52" s="8"/>
     </row>
-    <row r="53" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1663,7 +1799,7 @@
       <c r="M53"/>
       <c r="O53" s="8"/>
     </row>
-    <row r="54" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -1681,7 +1817,7 @@
       <c r="M54"/>
       <c r="O54" s="8"/>
     </row>
-    <row r="55" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>55</v>
       </c>
@@ -1699,7 +1835,7 @@
       <c r="M55"/>
       <c r="O55" s="8"/>
     </row>
-    <row r="56" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>56</v>
       </c>
@@ -1717,7 +1853,7 @@
       <c r="M56"/>
       <c r="O56" s="8"/>
     </row>
-    <row r="57" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>4</v>
       </c>
@@ -1747,57 +1883,642 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="10.75" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.796875" style="5" customWidth="1"/>
+    <col min="2" max="1024" width="10.69921875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-    </row>
-    <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-    </row>
-    <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-    </row>
-    <row r="4" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-    </row>
-    <row r="5" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-    </row>
-    <row r="6" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-    </row>
-    <row r="7" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-    </row>
-    <row r="9" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-    </row>
-    <row r="10" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+    <row r="1" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.1232" bottom="1.1232" header="0.78739999999999999" footer="0.78739999999999999"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;10Page &amp;P</oddFooter>
@@ -1806,14 +2527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="AMK1:XFD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="10.75" style="5" customWidth="1"/>
+    <col min="1" max="1024" width="10.69921875" style="5" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.1232" bottom="1.1232" header="0.78739999999999999" footer="0.78739999999999999"/>

</xml_diff>